<commit_message>
First commit - Moviescope project
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29203"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\PA1PEPF0011BBB8\EXCELCNV\0a26a6f0-6116-4648-b4b6-a6b789d47816\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Projet Simplon\react\moviescope\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69D90B2C-FD1A-4A1C-94ED-438609F59EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{987DA18F-84D2-4A6D-89A5-BD0A7B7085F6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="6890"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -581,26 +580,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -608,7 +607,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -616,7 +615,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -624,35 +623,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -660,7 +659,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -668,14 +667,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -683,14 +682,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -698,7 +697,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -706,14 +705,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -721,7 +720,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1077,49 +1076,49 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Lien hypertexte" xfId="42" builtinId="8"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1430,24 +1429,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFF9F13-2D58-4D5C-9A4B-670EFF4C7E2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.58203125" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="254.85546875" customWidth="1"/>
+    <col min="6" max="6" width="254.83203125" customWidth="1"/>
     <col min="7" max="7" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6">
+    <row r="2" spans="1:7" ht="182" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1493,7 +1492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="409.6">
+    <row r="3" spans="1:7" ht="154" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1516,7 +1515,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="409.6">
+    <row r="4" spans="1:7" ht="182" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="366">
+    <row r="5" spans="1:7" ht="140" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1562,7 +1561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="409.6">
+    <row r="6" spans="1:7" ht="168" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="409.6">
+    <row r="7" spans="1:7" ht="154" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1608,7 +1607,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="321">
+    <row r="8" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="167.25">
+    <row r="9" spans="1:7" ht="154" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="152.25">
+    <row r="10" spans="1:7" ht="140" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1677,7 +1676,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="152.25">
+    <row r="11" spans="1:7" ht="140" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1700,7 +1699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="137.25">
+    <row r="12" spans="1:7" ht="126" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1723,7 +1722,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="183">
+    <row r="13" spans="1:7" ht="154" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1746,7 +1745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="167.25">
+    <row r="14" spans="1:7" ht="154" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1769,7 +1768,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="167.25">
+    <row r="15" spans="1:7" ht="154" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1792,7 +1791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="121.5">
+    <row r="16" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1815,7 +1814,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="137.25">
+    <row r="17" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1838,7 +1837,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="91.5">
+    <row r="18" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1861,7 +1860,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="106.5">
+    <row r="19" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="91.5">
+    <row r="20" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1907,7 +1906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="152.25">
+    <row r="21" spans="1:7" ht="140" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1930,7 +1929,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="106.5">
+    <row r="22" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1953,7 +1952,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="121.5">
+    <row r="23" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1976,7 +1975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="106.5">
+    <row r="24" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="121.5">
+    <row r="25" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2022,7 +2021,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="152.25">
+    <row r="26" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2045,7 +2044,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="183">
+    <row r="27" spans="1:7" ht="154" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2068,7 +2067,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="167.25">
+    <row r="28" spans="1:7" ht="154" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="106.5">
+    <row r="29" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2114,7 +2113,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="152.25">
+    <row r="30" spans="1:7" ht="126" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="91.5">
+    <row r="31" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2160,7 +2159,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="121.5">
+    <row r="32" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2183,7 +2182,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="152.25">
+    <row r="33" spans="1:7" ht="126" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="121.5">
+    <row r="34" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2229,7 +2228,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="121.5">
+    <row r="35" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2252,7 +2251,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="91.5">
+    <row r="36" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="137.25">
+    <row r="37" spans="1:7" ht="126" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2298,7 +2297,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="137.25">
+    <row r="38" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2321,7 +2320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="121.5">
+    <row r="39" spans="1:7" ht="112" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2344,7 +2343,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="76.5">
+    <row r="40" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2367,7 +2366,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="76.5">
+    <row r="41" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2392,37 +2391,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{F4A15226-84BA-4B76-9C70-858CC7B83605}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{D78EF6F0-6B82-4335-AF21-B71FDE79236F}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{ACECB80A-7212-44AA-81BE-450FA63727B7}"/>
-    <hyperlink ref="E6" r:id="rId4" xr:uid="{CBBEF6F9-A4FA-4C3F-BFB7-447D58D3586F}"/>
-    <hyperlink ref="E8" r:id="rId5" xr:uid="{5DFF9D0F-1F36-4871-9EDE-DE58DD589644}"/>
-    <hyperlink ref="E9" r:id="rId6" xr:uid="{3E7CFF46-3525-4745-A6E7-A3431E20A35F}"/>
-    <hyperlink ref="E10" r:id="rId7" xr:uid="{78B590AB-3EE4-4389-8448-B168720A1960}"/>
-    <hyperlink ref="E11" r:id="rId8" xr:uid="{BEA2CE64-174F-4418-8BBB-AB2F4A95B0E2}"/>
-    <hyperlink ref="E13" r:id="rId9" xr:uid="{49DAC9E1-CF4E-4625-9CF1-0BEBF31E8A9A}"/>
-    <hyperlink ref="E14" r:id="rId10" xr:uid="{F57FCEBA-D122-469C-BCFD-F883DD510BBB}"/>
-    <hyperlink ref="E16" r:id="rId11" xr:uid="{77FDB78C-C458-46C3-A219-E5A63955485E}"/>
-    <hyperlink ref="E17" r:id="rId12" xr:uid="{7BDC23E6-4DEA-449F-9EEF-A4F37373F421}"/>
-    <hyperlink ref="E18" r:id="rId13" xr:uid="{175F2EE5-F8B1-497E-9200-78181ACC236F}"/>
-    <hyperlink ref="E19" r:id="rId14" xr:uid="{F4E50176-BBE3-4A96-ACAA-C5E902D82C46}"/>
-    <hyperlink ref="E20" r:id="rId15" xr:uid="{C8D43E64-9178-47B3-A122-DE936A5420CF}"/>
-    <hyperlink ref="E21" r:id="rId16" xr:uid="{8CB7619D-44D2-4096-BA08-B782C0F9025C}"/>
-    <hyperlink ref="E22" r:id="rId17" xr:uid="{F4476983-DD3A-4D2A-A2BE-621422211A18}"/>
-    <hyperlink ref="E24" r:id="rId18" xr:uid="{1CC900BF-A6F8-4550-BCED-4F86FE35C1EB}"/>
-    <hyperlink ref="E25" r:id="rId19" xr:uid="{B3E02855-0C93-43DF-8E6B-085230FC25B2}"/>
-    <hyperlink ref="E26" r:id="rId20" xr:uid="{9C011508-9AE8-4AEF-BD1E-475227C93561}"/>
-    <hyperlink ref="E27" r:id="rId21" xr:uid="{82E14FEE-00FD-4835-ACA6-CED97EE4E0C0}"/>
-    <hyperlink ref="E28" r:id="rId22" xr:uid="{05C0CD4A-0945-49E2-8887-EF1109D13EE8}"/>
-    <hyperlink ref="E29" r:id="rId23" xr:uid="{65F3B562-6E0E-405B-9D8D-ED41561FCD97}"/>
-    <hyperlink ref="E33" r:id="rId24" xr:uid="{150CF53F-A735-4F31-A398-8F0CAB167DFF}"/>
-    <hyperlink ref="E34" r:id="rId25" xr:uid="{27BFA7D7-20E7-468D-877B-196415318B98}"/>
-    <hyperlink ref="E35" r:id="rId26" xr:uid="{698286A1-2C24-4543-B231-70C1AE6FB2E7}"/>
-    <hyperlink ref="E36" r:id="rId27" xr:uid="{4990F8C9-86DF-407A-8B1F-0DBEC3295912}"/>
-    <hyperlink ref="E37" r:id="rId28" xr:uid="{27A829F6-7B13-4525-B0E5-6CD48038E5A4}"/>
-    <hyperlink ref="E38" r:id="rId29" xr:uid="{790E29A2-3733-4FD0-9653-238A55824B06}"/>
-    <hyperlink ref="E39" r:id="rId30" xr:uid="{A9C1C2AF-CAA8-445E-AFAC-0E62EBC3698D}"/>
-    <hyperlink ref="E41" r:id="rId31" xr:uid="{5845D15F-0B4D-477A-8C7F-541711D0D444}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E8" r:id="rId5"/>
+    <hyperlink ref="E9" r:id="rId6"/>
+    <hyperlink ref="E10" r:id="rId7"/>
+    <hyperlink ref="E11" r:id="rId8"/>
+    <hyperlink ref="E13" r:id="rId9"/>
+    <hyperlink ref="E14" r:id="rId10"/>
+    <hyperlink ref="E16" r:id="rId11"/>
+    <hyperlink ref="E17" r:id="rId12"/>
+    <hyperlink ref="E18" r:id="rId13"/>
+    <hyperlink ref="E19" r:id="rId14"/>
+    <hyperlink ref="E20" r:id="rId15"/>
+    <hyperlink ref="E21" r:id="rId16"/>
+    <hyperlink ref="E22" r:id="rId17"/>
+    <hyperlink ref="E24" r:id="rId18"/>
+    <hyperlink ref="E25" r:id="rId19"/>
+    <hyperlink ref="E26" r:id="rId20"/>
+    <hyperlink ref="E27" r:id="rId21"/>
+    <hyperlink ref="E28" r:id="rId22"/>
+    <hyperlink ref="E29" r:id="rId23"/>
+    <hyperlink ref="E33" r:id="rId24"/>
+    <hyperlink ref="E34" r:id="rId25"/>
+    <hyperlink ref="E35" r:id="rId26"/>
+    <hyperlink ref="E36" r:id="rId27"/>
+    <hyperlink ref="E37" r:id="rId28"/>
+    <hyperlink ref="E38" r:id="rId29"/>
+    <hyperlink ref="E39" r:id="rId30"/>
+    <hyperlink ref="E41" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>